<commit_message>
Update doc and example files.
</commit_message>
<xml_diff>
--- a/doc/SimpleExample01.xlsx
+++ b/doc/SimpleExample01.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jan\rdkit4excel\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="390" yWindow="30" windowWidth="19140" windowHeight="8730"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="RDKit examples" sheetId="1" r:id="rId1"/>
     <sheet name="Descriptor List" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -25,7 +20,7 @@
     <author>jan</author>
   </authors>
   <commentList>
-    <comment ref="H5" authorId="0" shapeId="0">
+    <comment ref="H5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -660,16 +655,16 @@
     <t>The function =rdkit_descriptor expects a SMILES string and the name of an RDKit function from the Descriptor module. Default descriptor used is "MolLogP".</t>
   </si>
   <si>
-    <t>The Function "=rdkit_version" returns the property rdkit_version from the COM automation server.</t>
-  </si>
-  <si>
-    <t>The Function "=rdkit_SmilesToMolBlock" converts a SMILES string to a MolBlock that can be rendered with Proteax For Spreadsheets. Rendering is automatically updated when SMILES input is changed.</t>
+    <t>The Function "=rdkit_smiles_to_molblock" converts a SMILES string to a MolBlock that can be rendered with Proteax For Spreadsheets. Rendering is automatically updated when SMILES input is changed.</t>
+  </si>
+  <si>
+    <t>The Function "=rdkit_info_version" returns the property rdkit_version from the COM automation server.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -720,13 +715,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -798,56 +790,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>351180</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1378559</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>901700</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="21" name="AF3839B4C95143669F2C59085B5A3271" descr="Proteax image 2055x1702">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1875180" y="1148080"/>
-          <a:ext cx="1027379" cy="850900"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>203618</xdr:rowOff>
@@ -863,7 +805,7 @@
         <xdr:cNvPr id="22" name="F86CFB5D2C4147D18534A977A9579174" descr="Proteax image 4682x1568">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -872,7 +814,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -913,7 +855,7 @@
         <xdr:cNvPr id="23" name="5B660B148CBA4E61A3D40A39218DB42D" descr="Proteax image 4362x2782">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -922,7 +864,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -963,7 +905,7 @@
         <xdr:cNvPr id="24" name="FCB73608CB9242388F2ED22F6F203BA3" descr="Proteax image 2630x1318">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -972,7 +914,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1013,10 +955,54 @@
         <xdr:cNvPr id="25" name="9AF889E37B554752AC5732F0AB0D52DC" descr="Proteax image 2975x1650">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000019000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1621771" y="4958080"/>
+          <a:ext cx="1534199" cy="850900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>210955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1635125</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>741545</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="71013ABD17B24679B94A5A8C6D06ADC5" descr="Proteax image 4682x1568"/>
         <xdr:cNvPicPr>
           <a:picLocks/>
         </xdr:cNvPicPr>
@@ -1035,8 +1021,184 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1621771" y="4958080"/>
+          <a:off x="1536700" y="3401830"/>
+          <a:ext cx="1584325" cy="530590"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>175884</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1510041</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>901700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="BF8C9D505DD847A2B8DECB530C53840D" descr="Proteax image 4362x2782"/>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1661784" y="4194175"/>
+          <a:ext cx="1334157" cy="850900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>329273</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1356652</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>901700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="7F6D8E7F798941A5AA32B57796553A60" descr="Proteax image 2055x1702"/>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1815173" y="2289175"/>
+          <a:ext cx="1027379" cy="850900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>75863</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1610062</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>901700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="8F0CBDF887EF4976869B94D2926D5873" descr="Proteax image 2975x1650"/>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1561763" y="6099175"/>
           <a:ext cx="1534199" cy="850900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>79265</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1635125</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>873235</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="1D2096C9C7F84542BAF6292FA45DA52E" descr="Proteax image 2630x1318"/>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1536700" y="5175140"/>
+          <a:ext cx="1584325" cy="793970"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1091,7 +1253,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1124,26 +1286,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1176,23 +1321,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1369,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1387,34 +1515,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
       <c r="K1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+      <c r="A2" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
       <c r="K2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="A3" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
       <c r="K3" t="s">
         <v>16</v>
       </c>
@@ -1424,7 +1552,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="str">
-        <f>_xll.Python.RDKitXL.rdkit_version()</f>
+        <f>_xll.Python.RDKitXL.rdkit_info_version()</f>
         <v>2017.03.1</v>
       </c>
       <c r="K4" t="s">
@@ -1449,7 +1577,7 @@
       <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -1462,7 +1590,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="1"/>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1470,28 +1598,58 @@
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2" t="e">
-        <f ca="1">_xll.ProteaxRendering.CellRenderer.PROTEAX_IMAGE("AF3839B4C95143669F2C59085B5A3271|MOL0FH3|F", _xll.Python.RDKitXL.rdkit_SmilesToMolBlock(A7))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C7" s="4">
+      <c r="B7" s="2" t="str">
+        <f>_xll.ProteaxRendering.CellRenderer.PROTEAX_IMAGE("7F6D8E7F798941A5AA32B57796553A60|MOL0FH3|F", _xll.Python.RDKitXL.rdkit_smiles_to_molblock(A7))</f>
+        <v xml:space="preserve">
+     RDKit          2D
+ 13 13  0  0  0  0  0  0  0  0999 V2000
+   -3.8123   -1.2868    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -2.6987   -0.2818    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -3.0122    1.1850    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
+   -1.2716   -0.7438    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
+   -0.1580    0.2612    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -0.4715    1.7281    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    0.6420    2.7330    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    2.0691    2.2711    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    2.3827    0.8043    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    1.2691   -0.2007    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    1.5826   -1.6676    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    3.0097   -2.1295    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
+    0.4690   -2.6725    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
+  1  2  1  0
+  2  3  2  0
+  2  4  1  0
+  4  5  1  0
+  5  6  2  0
+  6  7  1  0
+  7  8  2  0
+  8  9  1  0
+  9 10  2  0
+ 10 11  1  0
+ 11 12  2  0
+ 11 13  1  0
+ 10  5  1  0
+M  END
+</v>
+      </c>
+      <c r="C7" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A7,C$6)</f>
         <v>1.3101</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A7,D$6)</f>
         <v>180.15899999999996</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A7,E$6)</f>
         <v>3</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A7,F$6)</f>
         <v>1</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A7,H$6)</f>
         <v>3.0435273546341013</v>
       </c>
@@ -1500,28 +1658,90 @@
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="e">
-        <f ca="1">_xll.ProteaxRendering.CellRenderer.PROTEAX_IMAGE("F86CFB5D2C4147D18534A977A9579174|MOL0FH3|F", _xll.Python.RDKitXL.rdkit_SmilesToMolBlock(A8))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C8" s="4">
+      <c r="B8" s="2" t="str">
+        <f>_xll.ProteaxRendering.CellRenderer.PROTEAX_IMAGE("71013ABD17B24679B94A5A8C6D06ADC5|MOL0FH3|F", _xll.Python.RDKitXL.rdkit_smiles_to_molblock(A8))</f>
+        <v xml:space="preserve">
+     RDKit          2D
+ 28 30  0  0  0  0  0  0  0  0999 V2000
+   -2.2049   -0.8533    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -3.6688   -1.1804    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -4.6841   -0.0762    0.0000 N   0  0  0  0  0  0  0  0  0  0  0  0
+   -4.2355    1.3551    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -5.4581    2.2241    0.0000 N   0  0  0  0  0  0  0  0  0  0  0  0
+   -6.6624    1.3298    0.0000 N   0  0  0  0  0  0  0  0  0  0  0  0
+   -6.1840   -0.0919    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -7.0530   -1.3145    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -7.9220   -2.5372    0.0000 F   0  0  0  0  0  0  0  0  0  0  0  0
+   -8.2756   -0.4456    0.0000 F   0  0  0  0  0  0  0  0  0  0  0  0
+   -5.8303   -2.1835    0.0000 F   0  0  0  0  0  0  0  0  0  0  0  0
+   -2.7716    1.6823    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -1.7563    0.5781    0.0000 N   0  0  0  0  0  0  0  0  0  0  0  0
+   -0.2924    0.9052    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    0.1562    2.3366    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
+    0.7228   -0.1990    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    2.1867    0.1282    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    3.2020   -0.9760    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    4.6659   -0.6489    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    5.6812   -1.7531    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    7.1450   -1.4259    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    7.5937    0.0054    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    6.5784    1.1096    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    5.1145    0.7825    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    4.0992    1.8867    0.0000 F   0  0  0  0  0  0  0  0  0  0  0  0
+    9.0576    0.3326    0.0000 F   0  0  0  0  0  0  0  0  0  0  0  0
+    8.1603   -2.5301    0.0000 F   0  0  0  0  0  0  0  0  0  0  0  0
+    2.6354    1.5595    0.0000 N   0  0  0  0  0  0  0  0  0  0  0  0
+  1  2  1  0
+  2  3  1  0
+  3  4  1  0
+  4  5  2  0
+  5  6  1  0
+  6  7  2  0
+  7  8  1  0
+  8  9  1  0
+  8 10  1  0
+  8 11  1  0
+  4 12  1  0
+ 12 13  1  0
+ 13 14  1  0
+ 14 15  2  0
+ 14 16  1  0
+ 16 17  1  0
+ 17 18  1  0
+ 18 19  1  0
+ 19 20  2  0
+ 20 21  1  0
+ 21 22  2  0
+ 22 23  1  0
+ 23 24  2  0
+ 24 25  1  0
+ 22 26  1  0
+ 21 27  1  0
+ 17 28  1  0
+ 13  1  1  0
+  7  3  1  0
+ 24 19  1  0
+M  END
+</v>
+      </c>
+      <c r="C8" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A8,C$6)</f>
         <v>2.0165000000000002</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A8,D$6)</f>
         <v>407.3180000000001</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A8,E$6)</f>
         <v>5</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A8,F$6)</f>
         <v>1</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4">
+      <c r="G8" s="3"/>
+      <c r="H8" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A8,H$6)</f>
         <v>1.6262839581617268</v>
       </c>
@@ -1530,28 +1750,95 @@
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="2" t="e">
-        <f ca="1">_xll.ProteaxRendering.CellRenderer.PROTEAX_IMAGE("5B660B148CBA4E61A3D40A39218DB42D|MOL0FH3|F", _xll.Python.RDKitXL.rdkit_SmilesToMolBlock(A9))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C9" s="4">
+      <c r="B9" s="2" t="str">
+        <f>_xll.ProteaxRendering.CellRenderer.PROTEAX_IMAGE("BF8C9D505DD847A2B8DECB530C53840D|MOL0FH3|F", _xll.Python.RDKitXL.rdkit_smiles_to_molblock(A9))</f>
+        <v xml:space="preserve">
+     RDKit          2D
+ 30 33  0  0  0  0  0  0  0  0999 V2000
+   -9.1442   -1.7840    0.0000 F   0  0  0  0  0  0  0  0  0  0  0  0
+   -7.8181   -1.0830    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -7.7622    0.4160    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -6.4361    1.1170    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -5.1660    0.3192    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -5.2219   -1.1798    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -6.5480   -1.8809    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -3.8399    1.0202    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -3.7840    2.5192    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
+   -2.5697    0.2223    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -1.2436    0.9234    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    0.0266    0.1255    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    0.3605   -1.3369    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -0.4374   -2.6070    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
+    1.8229   -1.0029    0.0000 N   0  0  0  0  0  0  0  0  0  0  0  0
+    3.0931   -1.8008    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    3.0372   -3.2998    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    4.3073   -4.0977    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    5.6334   -3.3966    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    6.9036   -4.1945    0.0000 F   0  0  0  0  0  0  0  0  0  0  0  0
+    5.6893   -1.8976    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    4.4192   -1.0997    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    1.4889    0.4594    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    2.2868    1.7296    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    3.7858    1.6737    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    4.5837    2.9439    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    3.8826    4.2700    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    4.6805    5.5402    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
+    2.3837    4.3259    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    1.5858    3.0557    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+  1  2  1  0
+  2  3  2  0
+  3  4  1  0
+  4  5  2  0
+  5  6  1  0
+  6  7  2  0
+  5  8  1  0
+  8  9  1  1
+  8 10  1  0
+ 10 11  1  0
+ 12 11  1  6
+ 12 13  1  0
+ 13 14  2  0
+ 13 15  1  0
+ 15 16  1  0
+ 16 17  2  0
+ 17 18  1  0
+ 18 19  2  0
+ 19 20  1  0
+ 19 21  1  0
+ 21 22  2  0
+ 15 23  1  0
+ 23 24  1  1
+ 24 25  2  0
+ 25 26  1  0
+ 26 27  2  0
+ 27 28  1  0
+ 27 29  1  0
+ 29 30  2  0
+  7  2  1  0
+ 22 16  1  0
+ 30 24  1  0
+ 23 12  1  0
+M  END
+</v>
+      </c>
+      <c r="C9" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A9,C$6)</f>
         <v>4.8883000000000036</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A9,D$6)</f>
         <v>409.43200000000007</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A9,E$6)</f>
         <v>3</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A9,F$6)</f>
         <v>2</v>
       </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4">
+      <c r="G9" s="3"/>
+      <c r="H9" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A9,H$6)</f>
         <v>1.5460770899142344</v>
       </c>
@@ -1560,28 +1847,55 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="e">
-        <f ca="1">_xll.ProteaxRendering.CellRenderer.PROTEAX_IMAGE("FCB73608CB9242388F2ED22F6F203BA3|MOL0FH3|F", _xll.Python.RDKitXL.rdkit_SmilesToMolBlock(A10))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C10" s="4">
+      <c r="B10" s="2" t="str">
+        <f>_xll.ProteaxRendering.CellRenderer.PROTEAX_IMAGE("1D2096C9C7F84542BAF6292FA45DA52E|MOL0FH3|F", _xll.Python.RDKitXL.rdkit_smiles_to_molblock(A10))</f>
+        <v xml:space="preserve">
+     RDKit          2D
+ 12 11  0  0  0  0  0  0  0  0999 V2000
+    3.1906    0.7126    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    4.5609    0.1026    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
+    1.9771   -0.1691    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    2.1340   -1.6609    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
+    0.6067    0.4409    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    0.4498    1.9327    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
+   -0.6067   -0.4409    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -0.4498   -1.9327    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
+   -1.9771    0.1691    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -2.1340    1.6609    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
+   -3.1906   -0.7126    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -4.5609   -0.1026    0.0000 O   0  0  0  0  0  0  0  0  0  0  0  0
+  1  2  1  0
+  1  3  1  0
+  3  4  1  0
+  3  5  1  0
+  5  6  1  0
+  5  7  1  0
+  7  8  1  0
+  7  9  1  0
+  9 10  1  0
+  9 11  1  0
+ 11 12  1  0
+M  END
+</v>
+      </c>
+      <c r="C10" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A10,C$6)</f>
         <v>-3.5854000000000004</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A10,D$6)</f>
         <v>182.172</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A10,E$6)</f>
         <v>6</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A10,F$6)</f>
         <v>6</v>
       </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A10,H$6)</f>
         <v>3.9851644508585786</v>
       </c>
@@ -1590,52 +1904,80 @@
       <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2" t="e">
-        <f ca="1">_xll.ProteaxRendering.CellRenderer.PROTEAX_IMAGE("9AF889E37B554752AC5732F0AB0D52DC|MOL0FH3|F", _xll.Python.RDKitXL.rdkit_SmilesToMolBlock(A11))</f>
-        <v>#NAME?</v>
-      </c>
-      <c r="C11" s="4">
+      <c r="B11" s="2" t="str">
+        <f>_xll.ProteaxRendering.CellRenderer.PROTEAX_IMAGE("8F0CBDF887EF4976869B94D2926D5873|MOL0FH3|F", _xll.Python.RDKitXL.rdkit_smiles_to_molblock(A11))</f>
+        <v xml:space="preserve">
+     RDKit          2D
+ 22 23  0  0  0  0  0  0  0  0999 V2000
+   -0.7500   -2.5981    0.0000 Cl  0  0  0  0  0  0  0  0  0  0  0  0
+   -1.5000   -1.2990    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -3.0000   -1.2990    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -3.7500   -2.5981    0.0000 Cl  0  0  0  0  0  0  0  0  0  0  0  0
+   -3.7500   -0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -5.2500    0.0000    0.0000 Cl  0  0  0  0  0  0  0  0  0  0  0  0
+   -3.0000    1.2990    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -3.7500    2.5981    0.0000 Cl  0  0  0  0  0  0  0  0  0  0  0  0
+   -1.5000    1.2990    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+   -0.7500    2.5981    0.0000 Cl  0  0  0  0  0  0  0  0  0  0  0  0
+   -0.7500   -0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    0.7500   -0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    1.5000   -1.2990    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    0.7500   -2.5981    0.0000 Cl  0  0  0  0  0  0  0  0  0  0  0  0
+    3.0000   -1.2990    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    3.7500   -2.5981    0.0000 Cl  0  0  0  0  0  0  0  0  0  0  0  0
+    3.7500    0.0000    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    5.2500    0.0000    0.0000 Cl  0  0  0  0  0  0  0  0  0  0  0  0
+    3.0000    1.2990    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    3.7500    2.5981    0.0000 Cl  0  0  0  0  0  0  0  0  0  0  0  0
+    1.5000    1.2990    0.0000 C   0  0  0  0  0  0  0  0  0  0  0  0
+    0.7500    2.5981    0.0000 Cl  0  0  0  0  0  0  0  0  0  0  0  0
+  1  2  1  0
+  2  3  2  0
+  3  4  1  0
+  3  5  1  0
+  5  6  1  0
+  5  7  2  0
+  7  8  1  0
+  7  9  1  0
+  9 10  1  0
+  9 11  2  0
+ 11 12  1  0
+ 12 13  2  0
+ 13 14  1  0
+ 13 15  1  0
+ 15 16  1  0
+ 15 17  2  0
+ 17 18  1  0
+ 17 19  1  0
+ 19 20  1  0
+ 19 21  2  0
+ 21 22  1  0
+ 11  2  1  0
+ 21 12  1  0
+M  END
+</v>
+      </c>
+      <c r="C11" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A11,C$6)</f>
         <v>9.8875999999999991</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A11,D$6)</f>
         <v>498.66200000000026</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A11,E$6)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A11,F$6)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4">
+      <c r="G11" s="3"/>
+      <c r="H11" s="3">
         <f>_xll.Python.RDKitXL.rdkit_descriptor($A11,H$6)</f>
         <v>3.0269140714779517</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:11" ht="52.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="2"/>
-    </row>
-    <row r="17" spans="1:3" ht="63.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="2"/>
-    </row>
-    <row r="18" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="2"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-    </row>
-    <row r="20" spans="1:3" ht="164.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>